<commit_message>
basic prototype of making latex tables from form is complete!'
</commit_message>
<xml_diff>
--- a/fifth/Report_Generation_Form.xlsx
+++ b/fifth/Report_Generation_Form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enfxm\Desktop\Python Testing\Test Report Template\Test-Report-Generator\fifth\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27222B0B-BC00-46C8-A5B8-6105F97B17CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0496CA-E11B-4493-954B-A138F315AD7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1810,7 +1810,7 @@
   <dimension ref="A1:P17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2339,6 +2339,7 @@
     <mergeCell ref="I5:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>